<commit_message>
transport task has been completed
</commit_message>
<xml_diff>
--- a/Лаб_1_Задания_1и2.xlsx
+++ b/Лаб_1_Задания_1и2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Books\Маг_1_семестр\Системный анализ\Задания\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F047405F-08A0-4FBF-A752-693A453ADD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFA19E0-A628-4237-AAA0-102EDBB02889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A727DC9E-F722-49DC-A457-0749AFA7BCE4}"/>
   </bookViews>
@@ -18,47 +18,98 @@
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Лист1!$A$8:$D$8</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">Лист2!$B$17:$E$19</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Лист1!$A$8:$D$8</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Лист2!$B$17:$E$19</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Лист1!$A$10</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Лист2!$C$10</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Лист1!$K$4</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">Лист2!$D$10</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">Лист1!$K$5</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">Лист2!$E$10</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">Лист1!$K$6</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">Лист2!$F$10</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">Лист2!$H$6</definedName>
+    <definedName name="solver_lhs7" localSheetId="1" hidden="1">Лист2!$H$7</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">Лист2!$H$8</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">8</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Лист1!$A$13</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Лист2!$G$16</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel7" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel8" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">96</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">Лист2!$H$10</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">Лист1!$C$4</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">Лист2!$I$10</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">Лист1!$C$5</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">Лист2!$J$10</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">Лист1!$C$6</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">Лист2!$K$10</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">Лист2!$J$6</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">Лист2!$J$7</definedName>
+    <definedName name="solver_rhs8" localSheetId="1" hidden="1">Лист2!$J$8</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -70,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Виды рес-ов</t>
   </si>
@@ -183,6 +234,63 @@
   </si>
   <si>
     <t>Задача №2</t>
+  </si>
+  <si>
+    <t>Заводы</t>
+  </si>
+  <si>
+    <t>Объекты</t>
+  </si>
+  <si>
+    <t>Сумма запасов</t>
+  </si>
+  <si>
+    <t>Сумма расходов</t>
+  </si>
+  <si>
+    <t>Модель Задачи</t>
+  </si>
+  <si>
+    <t>Стоимость перевозки за единицу</t>
+  </si>
+  <si>
+    <t>Запасено</t>
+  </si>
+  <si>
+    <t>Вывезено</t>
+  </si>
+  <si>
+    <t>Потребности</t>
+  </si>
+  <si>
+    <t>Доставлено</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>План перевозок</t>
+  </si>
+  <si>
+    <t>Затраты на перевозку</t>
   </si>
 </sst>
 </file>
@@ -238,7 +346,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -307,11 +415,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -331,22 +492,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -420,15 +608,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>352425</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>362671</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>85992</xdr:rowOff>
+      <xdr:colOff>305521</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>143142</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -451,7 +639,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7391400" y="552450"/>
+          <a:off x="7334250" y="809625"/>
           <a:ext cx="5163271" cy="1914792"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -773,57 +961,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="K3" s="7" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="K3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="7"/>
+      <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="3">
         <v>60</v>
       </c>
@@ -845,10 +1033,10 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="3">
         <v>400</v>
       </c>
@@ -870,10 +1058,10 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="3">
         <v>128</v>
       </c>
@@ -908,12 +1096,12 @@
         <v>10</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -943,17 +1131,17 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="F9" s="7" t="s">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="F9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -974,11 +1162,11 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -988,12 +1176,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:I3"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="F9:I9"/>
     <mergeCell ref="A9:C9"/>
@@ -1002,6 +1184,12 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1010,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2261C6-B223-4454-A43F-E03EC27504D5}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1021,196 +1209,395 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="15"/>
+      <c r="C3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="15"/>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="3">
+        <v>50</v>
+      </c>
+      <c r="J6" s="3">
+        <f>SUM(B17:E17)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="3">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>7</v>
+      </c>
       <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="H7" s="3">
+        <v>100</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" ref="J7:J8" si="0">SUM(B18:E18)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="13">
+        <v>4</v>
+      </c>
+      <c r="D8" s="13">
+        <v>5</v>
+      </c>
+      <c r="E8" s="13">
+        <v>7</v>
+      </c>
+      <c r="F8" s="14">
+        <v>8</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="3">
+        <v>50</v>
+      </c>
+      <c r="J8" s="3">
+        <f>SUM(B19:E19)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C10" s="3">
+        <v>50</v>
+      </c>
+      <c r="D10" s="3">
+        <v>70</v>
+      </c>
+      <c r="E10" s="3">
+        <v>40</v>
+      </c>
+      <c r="F10" s="3">
+        <v>40</v>
+      </c>
       <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+      <c r="H10" s="3">
+        <f>SUM(B17:B19)</f>
+        <v>50</v>
+      </c>
+      <c r="I10" s="3">
+        <f>SUM(C17:C19)</f>
+        <v>70</v>
+      </c>
+      <c r="J10" s="3">
+        <f>SUM(D17:D19)</f>
+        <v>40</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" ref="I10:K10" si="1">SUM(E17:E19)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="2"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <f>H6+H7+H8</f>
+        <v>200</v>
+      </c>
+      <c r="C13" s="3">
+        <f>C10+D10+E10+F10</f>
+        <v>200</v>
+      </c>
+      <c r="E13" s="21" t="str">
+        <f>IF(A13=C13,"Закрытая","Открытая")</f>
+        <v>Закрытая</v>
+      </c>
+      <c r="F13" s="21"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-    </row>
-    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="3">
+        <f>SUMPRODUCT(C6:F8,B17:E19)</f>
+        <v>510</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="20">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3">
+        <v>40</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="20">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>70</v>
+      </c>
+      <c r="D18" s="3">
+        <v>30</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="20">
+        <v>50</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="19">
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="C3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>